<commit_message>
Make the masterCashierNPC excel better + removed the day and interaction from cashier interaction inspector
</commit_message>
<xml_diff>
--- a/Assets/Data/Excel/MasterCashierNPC.xlsx
+++ b/Assets/Data/Excel/MasterCashierNPC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_VincentGame\HorrorGame\Assets\Data\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF23564-0CDF-4FEA-B58D-F78E114D6949}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B50375D-3CEE-4688-9945-5EB079944B60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{CE5CDD7E-8CFD-476C-AB84-63CE99224655}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>id</t>
   </si>
@@ -49,6 +49,21 @@
   </si>
   <si>
     <t>Actor_NPC_01</t>
+  </si>
+  <si>
+    <t>interactionPath</t>
+  </si>
+  <si>
+    <t>Cashier_Interaction_Day01_01</t>
+  </si>
+  <si>
+    <t>Cashier_Interaction_Day01_02</t>
+  </si>
+  <si>
+    <t>Cashier_Interaction_Day02_01</t>
+  </si>
+  <si>
+    <t>Cashier_Interaction_Day02_02</t>
   </si>
 </sst>
 </file>
@@ -400,19 +415,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94E91137-7BD2-48ED-A93D-3ECC6F638E0D}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="16.5546875" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="28.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -425,8 +441,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -439,8 +458,11 @@
       <c r="D2" t="s">
         <v>4</v>
       </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -453,8 +475,11 @@
       <c r="D3" t="s">
         <v>4</v>
       </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -467,8 +492,11 @@
       <c r="D4" t="s">
         <v>4</v>
       </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -480,6 +508,9 @@
       </c>
       <c r="D5" t="s">
         <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Can slot in cashier interaction folder into definition without putting interaction in one by one + interaction path in MasterCashierNPC excel now uses the dayID and interactionID to minimize mistakes
</commit_message>
<xml_diff>
--- a/Assets/Data/Excel/MasterCashierNPC.xlsx
+++ b/Assets/Data/Excel/MasterCashierNPC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_VincentGame\HorrorGame\Assets\Data\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B50375D-3CEE-4688-9945-5EB079944B60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9395EF8-B1B8-4BA2-8AB8-7BBA96E2D113}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{CE5CDD7E-8CFD-476C-AB84-63CE99224655}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t>id</t>
   </si>
@@ -54,16 +54,16 @@
     <t>interactionPath</t>
   </si>
   <si>
-    <t>Cashier_Interaction_Day01_01</t>
-  </si>
-  <si>
-    <t>Cashier_Interaction_Day01_02</t>
-  </si>
-  <si>
-    <t>Cashier_Interaction_Day02_01</t>
-  </si>
-  <si>
-    <t>Cashier_Interaction_Day02_02</t>
+    <t>Cashier_Interaction_Day##_**</t>
+  </si>
+  <si>
+    <t>** is interactionID</t>
+  </si>
+  <si>
+    <t>## is dayID</t>
+  </si>
+  <si>
+    <t>AUTO</t>
   </si>
 </sst>
 </file>
@@ -415,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94E91137-7BD2-48ED-A93D-3ECC6F638E0D}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -426,9 +426,10 @@
     <col min="3" max="3" width="16.5546875" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="28.109375" customWidth="1"/>
+    <col min="9" max="9" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -445,7 +446,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -461,8 +462,11 @@
       <c r="E2" t="s">
         <v>6</v>
       </c>
+      <c r="I2" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -476,10 +480,13 @@
         <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="I3" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -493,10 +500,13 @@
         <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="I4" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -510,7 +520,7 @@
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>